<commit_message>
update scr post postprocessing
</commit_message>
<xml_diff>
--- a/ssp_modeling/scenario_mapping/Final scenario LULC areas_shared with SISEPUEDE.xlsx
+++ b/ssp_modeling/scenario_mapping/Final scenario LULC areas_shared with SISEPUEDE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tecmx-my.sharepoint.com/personal/cffuentes_tec_mx/Documents/SISEPUEDE/Uganda/lndu/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fabian_fuentes\repos\ssp_uganda\ssp_modeling\scenario_mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{0713378D-F1A5-4D87-A303-20C4EAD9CA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44B04649-EE7A-4128-8799-06563F36E8E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D2E687-2CE5-4D90-A6DB-D3AD954F606A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17110" yWindow="0" windowWidth="17380" windowHeight="13770" activeTab="1" xr2:uid="{2AEF5E3E-0A21-4B2E-B725-9AA9DDC8DE6E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{2AEF5E3E-0A21-4B2E-B725-9AA9DDC8DE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data for Diji" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data for Diji'!$A$4:$Q$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data for Diji'!$A$4:$R$17</definedName>
     <definedName name="DiscRate">'[1]Sustainability adjustment'!$C$3</definedName>
     <definedName name="Global2005_Ricke">[2]Carbon!$E$22</definedName>
     <definedName name="Global2005Rand">[2]Carbon!$F$22</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="59">
   <si>
     <t>Seanrio LULC areas</t>
   </si>
@@ -201,19 +201,51 @@
   </si>
   <si>
     <t>SISEPUEDE</t>
+  </si>
+  <si>
+    <t>Primary forests</t>
+  </si>
+  <si>
+    <t>Secondary forests</t>
+  </si>
+  <si>
+    <t>Name: 0, dtype: float64</t>
+  </si>
+  <si>
+    <t>pij_lndu_grasslands_to_wetlands</t>
+  </si>
+  <si>
+    <t>pij_lndu_grasslands_to_forests_mangroves</t>
+  </si>
+  <si>
+    <t>pij_lndu_grasslands_to_forests_secondary</t>
+  </si>
+  <si>
+    <t>pij_lndu_grasslands_to_croplands</t>
+  </si>
+  <si>
+    <t>pij_lndu_grasslands_to_other</t>
+  </si>
+  <si>
+    <t>pij_lndu_grasslands_to_grasslands</t>
+  </si>
+  <si>
+    <t>pij_lndu_grasslands_to_forests_primary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="172" formatCode="0.000000"/>
+    <numFmt numFmtId="173" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -243,6 +275,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="10">
@@ -301,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -329,13 +367,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -355,7 +402,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -380,13 +426,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -850,54 +905,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FF41A7-1AA5-4667-B7A2-8D546222A2A4}">
-  <dimension ref="A1:Q87"/>
+  <dimension ref="A1:V101"/>
   <sheetViews>
-    <sheetView zoomScale="92" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N5" sqref="N5:N12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="32.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.58203125" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="32.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.375" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="18.625" customWidth="1"/>
+    <col min="6" max="6" width="18.375" customWidth="1"/>
     <col min="7" max="10" width="16.75" customWidth="1"/>
-    <col min="12" max="12" width="30.58203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.4140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.375" customWidth="1"/>
+    <col min="14" max="14" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.625" customWidth="1"/>
+    <col min="16" max="16" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="38" t="s">
+    <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-    </row>
-    <row r="4" spans="1:17" ht="80" x14ac:dyDescent="0.4">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+    </row>
+    <row r="4" spans="1:19" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
@@ -928,27 +982,28 @@
       <c r="J4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="37" t="s">
+      <c r="M4" s="36" t="s">
         <v>48</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="11"/>
+      <c r="P4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="Q4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="R4" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3">
@@ -979,34 +1034,38 @@
         <f t="shared" ref="J5:J14" si="3">F5/F$17</f>
         <v>9.3190014271709434E-2</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="17">
         <v>0.167434</v>
       </c>
-      <c r="N5" s="35">
+      <c r="N5" s="34">
         <f>+G5+G12+G13</f>
         <v>0.54172938773883617</v>
       </c>
-      <c r="O5" s="35">
+      <c r="O5" s="34">
+        <f>+N5</f>
+        <v>0.54172938773883617</v>
+      </c>
+      <c r="P5" s="34">
         <f>+H5+H12+H13</f>
         <v>0.59798792185905869</v>
       </c>
-      <c r="P5" s="35">
+      <c r="Q5" s="34">
         <f>+I5+I12+I13</f>
         <v>0.67211360620840199</v>
       </c>
-      <c r="Q5" s="35">
+      <c r="R5" s="34">
         <f>+J5+J12+J13</f>
         <v>0.78792287693961527</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3">
@@ -1043,24 +1102,28 @@
       <c r="M6" s="4">
         <v>0</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="4">
         <v>0</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="4">
+        <f t="shared" ref="O6:O12" si="4">+N6</f>
         <v>0</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="4">
         <v>0</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3">
@@ -1091,34 +1154,38 @@
         <f t="shared" si="3"/>
         <v>3.9823217161954255E-3</v>
       </c>
-      <c r="L7" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" s="20">
+      <c r="L7" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" s="19">
         <v>0.49474299999999999</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7" s="34">
         <f>+G6</f>
         <v>2.5318034648191934E-2</v>
       </c>
-      <c r="O7" s="35">
+      <c r="O7" s="34">
+        <f t="shared" si="4"/>
+        <v>2.5318034648191934E-2</v>
+      </c>
+      <c r="P7" s="34">
         <f>+H6</f>
         <v>2.492489974204189E-2</v>
       </c>
-      <c r="P7" s="35">
+      <c r="Q7" s="34">
         <f>+I6</f>
         <v>2.4184984642556511E-2</v>
       </c>
-      <c r="Q7" s="35">
+      <c r="R7" s="34">
         <f>+J6</f>
         <v>2.2302888665755763E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3">
@@ -1149,34 +1216,38 @@
         <f t="shared" si="3"/>
         <v>4.9032094748936855E-2</v>
       </c>
-      <c r="L8" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="M8" s="27">
+      <c r="L8" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" s="26">
         <v>2.0045E-2</v>
       </c>
-      <c r="N8" s="35">
+      <c r="N8" s="34">
         <f>+G7+G8+G9</f>
         <v>0.11376517377271864</v>
       </c>
-      <c r="O8" s="35">
+      <c r="O8" s="34">
+        <f t="shared" si="4"/>
+        <v>0.11376517377271864</v>
+      </c>
+      <c r="P8" s="34">
         <f>+H7+H8+H9</f>
         <v>0.10131238113353408</v>
       </c>
-      <c r="P8" s="35">
+      <c r="Q8" s="34">
         <f>+I7+I8+I9</f>
         <v>8.6864184358756133E-2</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="R8" s="34">
         <f>+J7+J8+J9</f>
         <v>6.3665571213278135E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3">
@@ -1207,34 +1278,38 @@
         <f t="shared" si="3"/>
         <v>1.0651154748145859E-2</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="23">
+      <c r="M9" s="22">
         <v>0.17493700000000001</v>
       </c>
-      <c r="N9" s="35">
+      <c r="N9" s="34">
         <f>+G10</f>
         <v>0.26657822761190836</v>
       </c>
-      <c r="O9" s="35">
+      <c r="O9" s="34">
+        <f t="shared" si="4"/>
+        <v>0.26657822761190836</v>
+      </c>
+      <c r="P9" s="34">
         <f>+H10</f>
         <v>0.22263171058425274</v>
       </c>
-      <c r="P9" s="35">
+      <c r="Q9" s="34">
         <f>+I10</f>
         <v>0.17269599840985733</v>
       </c>
-      <c r="Q9" s="35">
+      <c r="R9" s="34">
         <f>+J10</f>
         <v>9.5977820356562479E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="3">
@@ -1265,30 +1340,34 @@
         <f t="shared" si="3"/>
         <v>9.5977820356562479E-2</v>
       </c>
-      <c r="L10" s="31" t="s">
+      <c r="L10" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="M10" s="32">
+      <c r="M10" s="31">
         <v>0.109055</v>
       </c>
-      <c r="N10" s="35">
+      <c r="N10" s="34">
         <f>+G16</f>
         <v>5.4755282077962469E-4</v>
       </c>
-      <c r="O10" s="35">
+      <c r="O10" s="34">
+        <f t="shared" si="4"/>
+        <v>5.4755282077962469E-4</v>
+      </c>
+      <c r="P10" s="34">
         <f>+H16</f>
         <v>5.4755282077962469E-4</v>
       </c>
-      <c r="P10" s="35">
+      <c r="Q10" s="34">
         <f>+I16</f>
         <v>5.4755282077962469E-4</v>
       </c>
-      <c r="Q10" s="35">
+      <c r="R10" s="34">
         <f>+J16</f>
         <v>5.4744151754816987E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1323,34 +1402,38 @@
         <f t="shared" si="3"/>
         <v>1.4604486214305022E-2</v>
       </c>
-      <c r="L11" s="28" t="s">
+      <c r="L11" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11" s="28">
         <v>1.4822E-2</v>
       </c>
-      <c r="N11" s="35">
+      <c r="N11" s="34">
         <f>+G14</f>
         <v>9.0432763784842746E-3</v>
       </c>
-      <c r="O11" s="35">
+      <c r="O11" s="34">
+        <f t="shared" si="4"/>
+        <v>9.0432763784842746E-3</v>
+      </c>
+      <c r="P11" s="34">
         <f>+H14</f>
         <v>1.1078385183703776E-2</v>
       </c>
-      <c r="P11" s="35">
+      <c r="Q11" s="34">
         <f>+I14</f>
         <v>1.2928515214051932E-2</v>
       </c>
-      <c r="Q11" s="35">
+      <c r="R11" s="34">
         <f>+J14</f>
         <v>1.4775641130623662E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="3">
@@ -1381,34 +1464,39 @@
         <f t="shared" si="3"/>
         <v>0.61217249267213991</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="L12" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="39">
         <v>1.8964000000000002E-2</v>
       </c>
-      <c r="N12" s="35">
+      <c r="N12" s="40">
         <f>+G11</f>
         <v>4.3018347029080979E-2</v>
       </c>
-      <c r="O12" s="35">
+      <c r="O12" s="40">
+        <f t="shared" si="4"/>
+        <v>4.3018347029080979E-2</v>
+      </c>
+      <c r="P12" s="40">
         <f>+H11</f>
         <v>4.151714867662918E-2</v>
       </c>
-      <c r="P12" s="35">
+      <c r="Q12" s="40">
         <f>+I11</f>
         <v>3.0665158345596386E-2</v>
       </c>
-      <c r="Q12" s="35">
+      <c r="R12" s="40">
         <f>+J11</f>
         <v>1.4604486214305022E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S12" s="41"/>
+    </row>
+    <row r="13" spans="1:19" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="3">
@@ -1439,32 +1527,36 @@
         <f t="shared" si="3"/>
         <v>8.2560369995765853E-2</v>
       </c>
-      <c r="M13" s="36">
-        <f>+SUM(M5:M12)</f>
+      <c r="M13" s="35">
+        <f t="shared" ref="M13:R13" si="5">+SUM(M5:M12)</f>
         <v>1</v>
       </c>
-      <c r="N13" s="36">
-        <f>+SUM(N5:N12)</f>
+      <c r="N13" s="35">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="O13" s="36">
-        <f>+SUM(O5:O12)</f>
+      <c r="O13" s="35">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P13" s="35">
+        <f t="shared" si="5"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="P13" s="36">
-        <f>+SUM(P5:P12)</f>
+      <c r="Q13" s="35">
+        <f t="shared" si="5"/>
         <v>0.99999999999999978</v>
       </c>
-      <c r="Q13" s="36">
-        <f>+SUM(Q5:Q12)</f>
+      <c r="R13" s="35">
+        <f t="shared" si="5"/>
         <v>0.99979672603768843</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="3">
@@ -1495,12 +1587,30 @@
         <f t="shared" si="3"/>
         <v>1.4775641130623662E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="L14" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="34">
+        <f t="shared" ref="P14:P21" si="6">+P5-N5</f>
+        <v>5.6258534120222525E-2</v>
+      </c>
+      <c r="Q14" s="34">
+        <f>+Q5-P5</f>
+        <v>7.4125684349343302E-2</v>
+      </c>
+      <c r="R14" s="34">
+        <f>+R5-Q5</f>
+        <v>0.11580927073121328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="32" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="3">
@@ -1527,12 +1637,27 @@
       <c r="J15" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="L15" t="s">
+        <v>40</v>
+      </c>
+      <c r="P15" s="34">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="34">
+        <f t="shared" ref="Q15:Q21" si="7">+Q6-P6</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="34">
+        <f t="shared" ref="R15" si="8">+R6-Q6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="33" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="3">
@@ -1563,8 +1688,26 @@
         <f>F16/F$17</f>
         <v>5.4744151754816987E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="L16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="34">
+        <f t="shared" si="6"/>
+        <v>-3.9313490615004373E-4</v>
+      </c>
+      <c r="Q16" s="34">
+        <f t="shared" si="7"/>
+        <v>-7.3991509948537898E-4</v>
+      </c>
+      <c r="R16" s="34">
+        <f t="shared" ref="R16" si="9">+R7-Q7</f>
+        <v>-1.8820959768007482E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>25</v>
@@ -1585,1066 +1728,1356 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="L17" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="34">
+        <f t="shared" si="6"/>
+        <v>-1.2452792639184557E-2</v>
+      </c>
+      <c r="Q17" s="34">
+        <f t="shared" si="7"/>
+        <v>-1.4448196774777947E-2</v>
+      </c>
+      <c r="R17" s="34">
+        <f t="shared" ref="R17" si="10">+R8-Q8</f>
+        <v>-2.3198613145477998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="39" t="s">
+      <c r="L18" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="34">
+        <f t="shared" si="6"/>
+        <v>-4.3946517027655618E-2</v>
+      </c>
+      <c r="Q18" s="34">
+        <f t="shared" si="7"/>
+        <v>-4.9935712174395408E-2</v>
+      </c>
+      <c r="R18" s="34">
+        <f t="shared" ref="R18" si="11">+R9-Q9</f>
+        <v>-7.6718178053294853E-2</v>
+      </c>
+      <c r="U18">
+        <v>2.24E-4</v>
+      </c>
+      <c r="V18">
+        <f>+U18</f>
+        <v>2.24E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="L19" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="34">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="34">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="34">
+        <f t="shared" ref="R19" si="12">+R10-Q10</f>
+        <v>-1.1130323145482415E-7</v>
+      </c>
+      <c r="T19" t="s">
+        <v>52</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="L20" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="34">
+        <f t="shared" si="6"/>
+        <v>2.0351088052195012E-3</v>
+      </c>
+      <c r="Q20" s="34">
+        <f t="shared" si="7"/>
+        <v>1.8501300303481565E-3</v>
+      </c>
+      <c r="R20" s="34">
+        <f t="shared" ref="R20" si="13">+R11-Q11</f>
+        <v>1.8471259165717298E-3</v>
+      </c>
+      <c r="T20" t="s">
+        <v>53</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="L21" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="34">
+        <f t="shared" si="6"/>
+        <v>-1.5011983524517991E-3</v>
+      </c>
+      <c r="Q21" s="34">
+        <f t="shared" si="7"/>
+        <v>-1.0851990331032794E-2</v>
+      </c>
+      <c r="R21" s="34">
+        <f t="shared" ref="R21" si="14">+R12-Q12</f>
+        <v>-1.6060672131291365E-2</v>
+      </c>
+      <c r="T21" t="s">
+        <v>54</v>
+      </c>
+      <c r="U21">
+        <v>2.1220000000000002E-3</v>
+      </c>
+      <c r="V21">
+        <f>+U21</f>
+        <v>2.1220000000000002E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="P22" s="34"/>
+      <c r="T22" t="s">
+        <v>55</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="L23" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="N23" s="35"/>
+      <c r="P23" s="45">
+        <f>100%+P18</f>
+        <v>0.95605348297234438</v>
+      </c>
+      <c r="Q23" s="45">
+        <f>100%+Q18</f>
+        <v>0.95006428782560459</v>
+      </c>
+      <c r="R23" s="45">
+        <f>100%+R18</f>
+        <v>0.92328182194670516</v>
+      </c>
+      <c r="T23" t="s">
+        <v>56</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="L24" t="s">
+        <v>40</v>
+      </c>
+      <c r="T24" t="s">
+        <v>57</v>
+      </c>
+      <c r="U24">
+        <v>0.99765400000000004</v>
+      </c>
+      <c r="V24">
+        <f>+U24-0.5</f>
+        <v>0.49765400000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="L25" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="S25" s="46"/>
+      <c r="T25" t="s">
+        <v>58</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="L26" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="P26" s="44"/>
+      <c r="T26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="L27" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="L28" s="30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="L29" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="L30" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-    </row>
-    <row r="20" spans="1:10" ht="48" x14ac:dyDescent="0.4">
-      <c r="A20" s="11" t="s">
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+    </row>
+    <row r="34" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B34" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D34" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E34" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F34" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G34" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H34" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I34" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J34" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A21" s="1">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C35" s="3">
         <v>329069</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D35" s="3">
         <v>668558</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E35" s="3">
         <v>668558</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F35" s="3">
         <v>668558</v>
       </c>
-      <c r="G21" s="4">
-        <f>C21/C$17</f>
+      <c r="G35" s="4">
+        <f>C35/C$17</f>
         <v>1.609061075023489E-2</v>
       </c>
-      <c r="H21" s="4">
-        <f>D21/D$17</f>
+      <c r="H35" s="4">
+        <f>D35/D$17</f>
         <v>3.2690732162420459E-2</v>
       </c>
-      <c r="I21" s="4">
-        <f t="shared" ref="I21:J30" si="4">E21/E$17</f>
+      <c r="I35" s="4">
+        <f t="shared" ref="I35:J44" si="15">E35/E$17</f>
         <v>3.2690732162420459E-2</v>
       </c>
-      <c r="J21" s="4">
-        <f t="shared" si="4"/>
+      <c r="J35" s="4">
+        <f t="shared" si="15"/>
         <v>3.2684086987762935E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A22" s="1">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>3</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C36" s="3">
         <v>517779</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D36" s="3">
         <v>517779</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E36" s="3">
         <v>517779</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F36" s="3">
         <v>2417779</v>
       </c>
-      <c r="G22" s="4">
-        <f t="shared" ref="G22:H30" si="5">C22/C$17</f>
+      <c r="G36" s="4">
+        <f t="shared" ref="G36:H44" si="16">C36/C$17</f>
         <v>2.5318034648191934E-2</v>
       </c>
-      <c r="H22" s="4">
-        <f t="shared" si="5"/>
+      <c r="H36" s="4">
+        <f t="shared" si="16"/>
         <v>2.5318034648191934E-2</v>
       </c>
-      <c r="I22" s="4">
-        <f t="shared" si="4"/>
+      <c r="I36" s="4">
+        <f t="shared" si="15"/>
         <v>2.5318034648191934E-2</v>
       </c>
-      <c r="J22" s="4">
-        <f t="shared" si="4"/>
+      <c r="J36" s="4">
+        <f t="shared" si="15"/>
         <v>0.11819901811538638</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A23" s="1">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>4</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C37" s="3">
         <v>153313</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D37" s="3">
         <v>2053313</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E37" s="3">
         <v>2053313</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F37" s="3">
         <v>153313</v>
       </c>
-      <c r="G23" s="4">
-        <f t="shared" si="5"/>
+      <c r="G37" s="4">
+        <f t="shared" si="16"/>
         <v>7.4966034659927306E-3</v>
       </c>
-      <c r="H23" s="4">
-        <f t="shared" si="5"/>
+      <c r="H37" s="4">
+        <f t="shared" si="16"/>
         <v>0.10040161860095316</v>
       </c>
-      <c r="I23" s="4">
-        <f t="shared" si="4"/>
+      <c r="I37" s="4">
+        <f t="shared" si="15"/>
         <v>0.10040161860095316</v>
       </c>
-      <c r="J23" s="4">
-        <f t="shared" si="4"/>
+      <c r="J37" s="4">
+        <f t="shared" si="15"/>
         <v>7.495079601702319E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A24" s="1">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>5</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C38" s="3">
         <v>1710720</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D38" s="3">
         <v>1710720</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E38" s="3">
         <v>1710720</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F38" s="3">
         <v>1710720</v>
       </c>
-      <c r="G24" s="4">
-        <f t="shared" si="5"/>
+      <c r="G38" s="4">
+        <f t="shared" si="16"/>
         <v>8.3649719732462893E-2</v>
       </c>
-      <c r="H24" s="4">
-        <f t="shared" si="5"/>
+      <c r="H38" s="4">
+        <f t="shared" si="16"/>
         <v>8.3649719732462893E-2</v>
       </c>
-      <c r="I24" s="4">
-        <f t="shared" si="4"/>
+      <c r="I38" s="4">
+        <f t="shared" si="15"/>
         <v>8.3649719732462893E-2</v>
       </c>
-      <c r="J24" s="4">
-        <f t="shared" si="4"/>
+      <c r="J38" s="4">
+        <f t="shared" si="15"/>
         <v>8.3632715922486625E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A25" s="1">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>6</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C39" s="3">
         <v>462578</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D39" s="3">
         <v>410184</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E39" s="3">
         <v>394217</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F39" s="3">
         <v>381525</v>
       </c>
-      <c r="G25" s="4">
-        <f t="shared" si="5"/>
+      <c r="G39" s="4">
+        <f t="shared" si="16"/>
         <v>2.2618850574263012E-2</v>
       </c>
-      <c r="H25" s="4">
-        <f t="shared" si="5"/>
+      <c r="H39" s="4">
+        <f t="shared" si="16"/>
         <v>2.0056921435851898E-2</v>
       </c>
-      <c r="I25" s="4">
-        <f t="shared" si="4"/>
+      <c r="I39" s="4">
+        <f t="shared" si="15"/>
         <v>1.9276177027083525E-2</v>
       </c>
-      <c r="J25" s="4">
-        <f t="shared" si="4"/>
+      <c r="J39" s="4">
+        <f t="shared" si="15"/>
         <v>1.8651779334038714E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A26" s="1">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>7</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C40" s="3">
         <v>5451790</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D40" s="3">
         <v>4117488</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E40" s="3">
         <v>3873280</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F40" s="3">
         <v>3616939</v>
       </c>
-      <c r="G26" s="4">
-        <f t="shared" si="5"/>
+      <c r="G40" s="4">
+        <f t="shared" si="16"/>
         <v>0.26657822761190836</v>
       </c>
-      <c r="H26" s="4">
-        <f t="shared" si="5"/>
+      <c r="H40" s="4">
+        <f t="shared" si="16"/>
         <v>0.20133436050421996</v>
       </c>
-      <c r="I26" s="4">
-        <f t="shared" si="4"/>
+      <c r="I40" s="4">
+        <f t="shared" si="15"/>
         <v>0.18939323001154712</v>
       </c>
-      <c r="J26" s="4">
-        <f t="shared" si="4"/>
+      <c r="J40" s="4">
+        <f t="shared" si="15"/>
         <v>0.17682287685650652</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A27" s="1">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>8</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C41" s="3">
         <v>879768</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D41" s="3">
         <v>1186018</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E41" s="3">
         <v>1186018</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F41" s="3">
         <v>1186018</v>
       </c>
-      <c r="G27" s="4">
-        <f t="shared" si="5"/>
+      <c r="G41" s="4">
+        <f t="shared" si="16"/>
         <v>4.3018347029080979E-2</v>
       </c>
-      <c r="H27" s="4">
-        <f t="shared" si="5"/>
+      <c r="H41" s="4">
+        <f t="shared" si="16"/>
         <v>5.7993168547545E-2</v>
       </c>
-      <c r="I27" s="4">
-        <f t="shared" si="4"/>
+      <c r="I41" s="4">
+        <f t="shared" si="15"/>
         <v>5.7993168547545E-2</v>
       </c>
-      <c r="J27" s="4">
-        <f t="shared" si="4"/>
+      <c r="J41" s="4">
+        <f t="shared" si="15"/>
         <v>5.7981380046387331E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A28" s="1">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>9</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C42" s="3">
         <v>10580943</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D42" s="3">
         <v>9193185</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E42" s="3">
         <v>9015951</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F42" s="3">
         <v>8401173</v>
       </c>
-      <c r="G28" s="4">
-        <f t="shared" si="5"/>
+      <c r="G42" s="4">
+        <f t="shared" si="16"/>
         <v>0.51738035239850189</v>
       </c>
-      <c r="H28" s="4">
-        <f t="shared" si="5"/>
+      <c r="H42" s="4">
+        <f t="shared" si="16"/>
         <v>0.44952262713867958</v>
       </c>
-      <c r="I28" s="4">
-        <f t="shared" si="4"/>
+      <c r="I42" s="4">
+        <f t="shared" si="15"/>
         <v>0.4408563495321377</v>
       </c>
-      <c r="J28" s="4">
-        <f t="shared" si="4"/>
+      <c r="J42" s="4">
+        <f t="shared" si="15"/>
         <v>0.41071181427975628</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A29" s="1">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>10</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C43" s="3">
         <v>168893</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D43" s="3">
         <v>356069</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E43" s="3">
         <v>755641</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F43" s="3">
         <v>1601453</v>
       </c>
-      <c r="G29" s="4">
-        <f t="shared" si="5"/>
+      <c r="G43" s="4">
+        <f t="shared" si="16"/>
         <v>8.2584245900994054E-3</v>
       </c>
-      <c r="H29" s="4">
-        <f t="shared" si="5"/>
+      <c r="H43" s="4">
+        <f t="shared" si="16"/>
         <v>1.7410839912679065E-2</v>
       </c>
-      <c r="I29" s="4">
-        <f t="shared" si="4"/>
+      <c r="I43" s="4">
+        <f t="shared" si="15"/>
         <v>3.6948862390314016E-2</v>
       </c>
-      <c r="J29" s="4">
-        <f t="shared" si="4"/>
+      <c r="J43" s="4">
+        <f t="shared" si="15"/>
         <v>7.8290932363106747E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A30" s="1">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>11</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C44" s="3">
         <v>184944</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D44" s="3">
         <v>226483</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E44" s="3">
         <v>264320</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F44" s="3">
         <v>302319</v>
       </c>
-      <c r="G30" s="4">
-        <f t="shared" si="5"/>
+      <c r="G44" s="4">
+        <f t="shared" si="16"/>
         <v>9.0432763784842746E-3</v>
       </c>
-      <c r="H30" s="4">
-        <f t="shared" si="5"/>
+      <c r="H44" s="4">
+        <f t="shared" si="16"/>
         <v>1.1074424496216444E-2</v>
       </c>
-      <c r="I30" s="4">
-        <f t="shared" si="4"/>
+      <c r="I44" s="4">
+        <f t="shared" si="15"/>
         <v>1.2924554526564601E-2</v>
       </c>
-      <c r="J30" s="4">
-        <f t="shared" si="4"/>
+      <c r="J44" s="4">
+        <f t="shared" si="15"/>
         <v>1.4779601013006356E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A31" s="1">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>12</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C45" s="3">
         <v>3693693</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D45" s="3">
         <v>3693693</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E45" s="3">
         <v>3693693</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F45" s="3">
         <v>3693693</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G45" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H45" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I45" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J45" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A32" s="2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>13</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C46" s="3">
         <v>11198</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D46" s="3">
         <v>11198</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E46" s="3">
         <v>11198</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F46" s="3">
         <v>11198</v>
       </c>
-      <c r="G32" s="4">
-        <f t="shared" ref="G32:J32" si="6">C32/C$17</f>
+      <c r="G46" s="4">
+        <f t="shared" ref="G46:J46" si="17">C46/C$17</f>
         <v>5.4755282077962469E-4</v>
       </c>
-      <c r="H32" s="4">
-        <f t="shared" si="6"/>
+      <c r="H46" s="4">
+        <f t="shared" si="17"/>
         <v>5.4755282077962469E-4</v>
       </c>
-      <c r="I32" s="4">
-        <f t="shared" si="6"/>
+      <c r="I46" s="4">
+        <f t="shared" si="17"/>
         <v>5.4755282077962469E-4</v>
       </c>
-      <c r="J32" s="4">
-        <f t="shared" si="6"/>
+      <c r="J46" s="4">
+        <f t="shared" si="17"/>
         <v>5.4744151754816987E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C47" s="6">
         <v>20450995</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D47" s="6">
         <v>20450995</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E47" s="6">
         <v>20450995</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F47" s="6">
         <v>20455153</v>
       </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="38" t="s">
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
-    </row>
-    <row r="36" spans="1:10" ht="48" x14ac:dyDescent="0.4">
-      <c r="A36" s="11" t="s">
+      <c r="B49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="42"/>
+      <c r="J49" s="42"/>
+    </row>
+    <row r="50" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B50" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C50" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D50" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E50" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F50" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G50" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H36" s="11" t="s">
+      <c r="H50" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I36" s="11" t="s">
+      <c r="I50" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J36" s="11" t="s">
+      <c r="J50" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A37" s="1">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>1</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C51" s="3">
         <v>329069</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D51" s="3">
         <v>456400</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E51" s="3">
         <v>594500</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F51" s="3">
         <v>608054</v>
       </c>
-      <c r="G37" s="4">
-        <f>C37/C$17</f>
+      <c r="G51" s="4">
+        <f>C51/C$17</f>
         <v>1.609061075023489E-2</v>
       </c>
-      <c r="H37" s="4">
-        <f>D37/D$17</f>
+      <c r="H51" s="4">
+        <f>D51/D$17</f>
         <v>2.2316762582945231E-2</v>
       </c>
-      <c r="I37" s="4">
-        <f t="shared" ref="I37:J46" si="7">E37/E$17</f>
+      <c r="I51" s="4">
+        <f t="shared" ref="I51:J60" si="18">E51/E$17</f>
         <v>2.9069490261965248E-2</v>
       </c>
-      <c r="J37" s="4">
-        <f t="shared" si="7"/>
+      <c r="J51" s="4">
+        <f t="shared" si="18"/>
         <v>2.9726201510201365E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A38" s="1">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>3</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C52" s="3">
         <v>517779</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D52" s="3">
         <v>516957</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E52" s="3">
         <v>735206</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F52" s="3">
         <v>2515757</v>
       </c>
-      <c r="G38" s="4">
-        <f t="shared" ref="G38:H46" si="8">C38/C$17</f>
+      <c r="G52" s="4">
+        <f t="shared" ref="G52:H60" si="19">C52/C$17</f>
         <v>2.5318034648191934E-2</v>
       </c>
-      <c r="H38" s="4">
-        <f t="shared" si="8"/>
+      <c r="H52" s="4">
+        <f t="shared" si="19"/>
         <v>2.5277841004801967E-2</v>
       </c>
-      <c r="I38" s="4">
-        <f t="shared" si="7"/>
+      <c r="I52" s="4">
+        <f t="shared" si="18"/>
         <v>3.5949644503849326E-2</v>
       </c>
-      <c r="J38" s="4">
-        <f t="shared" si="7"/>
+      <c r="J52" s="4">
+        <f t="shared" si="18"/>
         <v>0.12298891140046715</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A39" s="1">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>4</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C53" s="3">
         <v>153313</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D53" s="3">
         <v>2053678</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E53" s="3">
         <v>2051774</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F53" s="3">
         <v>153678</v>
       </c>
-      <c r="G39" s="4">
-        <f t="shared" si="8"/>
+      <c r="G53" s="4">
+        <f t="shared" si="19"/>
         <v>7.4966034659927306E-3</v>
       </c>
-      <c r="H39" s="4">
-        <f t="shared" si="8"/>
+      <c r="H53" s="4">
+        <f t="shared" si="19"/>
         <v>0.10041946614333434</v>
       </c>
-      <c r="I39" s="4">
-        <f t="shared" si="7"/>
+      <c r="I53" s="4">
+        <f t="shared" si="18"/>
         <v>0.10032636553869384</v>
       </c>
-      <c r="J39" s="4">
-        <f t="shared" si="7"/>
+      <c r="J53" s="4">
+        <f t="shared" si="18"/>
         <v>7.5129235161428519E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A40" s="1">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>5</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C54" s="3">
         <v>1710720</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D54" s="3">
         <v>1679564</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E54" s="3">
         <v>1677834</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F54" s="3">
         <v>1710861</v>
       </c>
-      <c r="G40" s="4">
-        <f t="shared" si="8"/>
+      <c r="G54" s="4">
+        <f t="shared" si="19"/>
         <v>8.3649719732462893E-2</v>
       </c>
-      <c r="H40" s="4">
-        <f t="shared" si="8"/>
+      <c r="H54" s="4">
+        <f t="shared" si="19"/>
         <v>8.2126273073755085E-2</v>
       </c>
-      <c r="I40" s="4">
-        <f t="shared" si="7"/>
+      <c r="I54" s="4">
+        <f t="shared" si="18"/>
         <v>8.2041680612605888E-2</v>
       </c>
-      <c r="J40" s="4">
-        <f t="shared" si="7"/>
+      <c r="J54" s="4">
+        <f t="shared" si="18"/>
         <v>8.3639609051078714E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A41" s="1">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>6</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C55" s="3">
         <v>462578</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D55" s="3">
         <v>447507</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E55" s="3">
         <v>440162</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F55" s="3">
         <v>445402</v>
       </c>
-      <c r="G41" s="4">
-        <f t="shared" si="8"/>
+      <c r="G55" s="4">
+        <f t="shared" si="19"/>
         <v>2.2618850574263012E-2</v>
       </c>
-      <c r="H41" s="4">
-        <f t="shared" si="8"/>
+      <c r="H55" s="4">
+        <f t="shared" si="19"/>
         <v>2.1881918214737228E-2</v>
       </c>
-      <c r="I41" s="4">
-        <f t="shared" si="7"/>
+      <c r="I55" s="4">
+        <f t="shared" si="18"/>
         <v>2.1522766985176026E-2</v>
       </c>
-      <c r="J41" s="4">
-        <f t="shared" si="7"/>
+      <c r="J55" s="4">
+        <f t="shared" si="18"/>
         <v>2.1774562136005534E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A42" s="1">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>7</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C56" s="3">
         <v>5451790</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D56" s="3">
         <v>4878001</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E56" s="3">
         <v>4786034</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F56" s="3">
         <v>4852641</v>
       </c>
-      <c r="G42" s="4">
-        <f t="shared" si="8"/>
+      <c r="G56" s="4">
+        <f t="shared" si="19"/>
         <v>0.26657822761190836</v>
       </c>
-      <c r="H42" s="4">
-        <f t="shared" si="8"/>
+      <c r="H56" s="4">
+        <f t="shared" si="19"/>
         <v>0.23852145091229057</v>
       </c>
-      <c r="I42" s="4">
-        <f t="shared" si="7"/>
+      <c r="I56" s="4">
+        <f t="shared" si="18"/>
         <v>0.23402450589812379</v>
       </c>
-      <c r="J42" s="4">
-        <f t="shared" si="7"/>
+      <c r="J56" s="4">
+        <f t="shared" si="18"/>
         <v>0.23723318031402649</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A43" s="1">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>8</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C57" s="3">
         <v>879768</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D57" s="3">
         <v>1180013</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E57" s="3">
         <v>1278007</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F57" s="3">
         <v>1285149</v>
       </c>
-      <c r="G43" s="4">
-        <f t="shared" si="8"/>
+      <c r="G57" s="4">
+        <f t="shared" si="19"/>
         <v>4.3018347029080979E-2</v>
       </c>
-      <c r="H43" s="4">
-        <f t="shared" si="8"/>
+      <c r="H57" s="4">
+        <f t="shared" si="19"/>
         <v>5.7699539802342138E-2</v>
       </c>
-      <c r="I43" s="4">
-        <f t="shared" si="7"/>
+      <c r="I57" s="4">
+        <f t="shared" si="18"/>
         <v>6.2491189303992299E-2</v>
       </c>
-      <c r="J43" s="4">
-        <f t="shared" si="7"/>
+      <c r="J57" s="4">
+        <f t="shared" si="18"/>
         <v>6.2827640546125468E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A44" s="1">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>9</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C58" s="3">
         <v>10580943</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D58" s="3">
         <v>8629125</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E58" s="3">
         <v>7800440</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F58" s="3">
         <v>6798098</v>
       </c>
-      <c r="G44" s="4">
-        <f t="shared" si="8"/>
+      <c r="G58" s="4">
+        <f t="shared" si="19"/>
         <v>0.51738035239850189</v>
       </c>
-      <c r="H44" s="4">
-        <f t="shared" si="8"/>
+      <c r="H58" s="4">
+        <f t="shared" si="19"/>
         <v>0.42194157301392915</v>
       </c>
-      <c r="I44" s="4">
-        <f t="shared" si="7"/>
+      <c r="I58" s="4">
+        <f t="shared" si="18"/>
         <v>0.38142105066281617</v>
       </c>
-      <c r="J44" s="4">
-        <f t="shared" si="7"/>
+      <c r="J58" s="4">
+        <f t="shared" si="18"/>
         <v>0.33234158649412204</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A45" s="1">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>10</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C59" s="3">
         <v>168893</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D59" s="3">
         <v>354288</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E59" s="3">
         <v>757555</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F59" s="3">
         <v>1623696</v>
       </c>
-      <c r="G45" s="4">
-        <f t="shared" si="8"/>
+      <c r="G59" s="4">
+        <f t="shared" si="19"/>
         <v>8.2584245900994054E-3</v>
       </c>
-      <c r="H45" s="4">
-        <f t="shared" si="8"/>
+      <c r="H59" s="4">
+        <f t="shared" si="19"/>
         <v>1.7323753685334137E-2</v>
       </c>
-      <c r="I45" s="4">
-        <f t="shared" si="7"/>
+      <c r="I59" s="4">
+        <f t="shared" si="18"/>
         <v>3.7042451968718394E-2</v>
       </c>
-      <c r="J45" s="4">
-        <f t="shared" si="7"/>
+      <c r="J59" s="4">
+        <f t="shared" si="18"/>
         <v>7.9378335620369112E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A46" s="1">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>11</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C60" s="3">
         <v>184944</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D60" s="3">
         <v>249986</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E60" s="3">
         <v>324534</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F60" s="3">
         <v>450618</v>
       </c>
-      <c r="G46" s="4">
-        <f t="shared" si="8"/>
+      <c r="G60" s="4">
+        <f t="shared" si="19"/>
         <v>9.0432763784842746E-3</v>
       </c>
-      <c r="H46" s="4">
-        <f t="shared" si="8"/>
+      <c r="H60" s="4">
+        <f t="shared" si="19"/>
         <v>1.2223659533435904E-2</v>
       </c>
-      <c r="I46" s="4">
-        <f t="shared" si="7"/>
+      <c r="I60" s="4">
+        <f t="shared" si="18"/>
         <v>1.5868861148320656E-2</v>
       </c>
-      <c r="J46" s="4">
-        <f t="shared" si="7"/>
+      <c r="J60" s="4">
+        <f t="shared" si="18"/>
         <v>2.2029559006476265E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A47" s="1">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>12</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C61" s="3">
         <v>3693693</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D61" s="3">
         <v>3688730</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E61" s="3">
         <v>3688374</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F61" s="3">
         <v>3693793</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="G61" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="H61" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="I61" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="J61" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A48" s="2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
         <v>13</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C62" s="3">
         <v>11198</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D62" s="3">
         <v>10439</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E62" s="3">
         <v>10268</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F62" s="3">
         <v>11199</v>
       </c>
-      <c r="G48" s="4">
-        <f t="shared" ref="G48:J48" si="9">C48/C$17</f>
+      <c r="G62" s="4">
+        <f t="shared" ref="G62:J62" si="20">C62/C$17</f>
         <v>5.4755282077962469E-4</v>
       </c>
-      <c r="H48" s="4">
-        <f t="shared" si="9"/>
+      <c r="H62" s="4">
+        <f t="shared" si="20"/>
         <v>5.1043971210202731E-4</v>
       </c>
-      <c r="I48" s="4">
-        <f t="shared" si="9"/>
+      <c r="I62" s="4">
+        <f t="shared" si="20"/>
         <v>5.0207826073988084E-4</v>
       </c>
-      <c r="J48" s="4">
-        <f t="shared" si="9"/>
+      <c r="J62" s="4">
+        <f t="shared" si="20"/>
         <v>5.4749040498499322E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5" t="s">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C63" s="6">
         <v>20450995</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D63" s="6">
         <v>20455958</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E63" s="6">
         <v>20456314</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F63" s="6">
         <v>20455153</v>
       </c>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A68" s="1"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A71" s="1"/>
-      <c r="C71" s="9"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A72" s="1"/>
-      <c r="C72" s="9"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A73" s="1"/>
-      <c r="C73" s="9"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.4">
-      <c r="D81" s="10"/>
-    </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.4">
-      <c r="D82" s="10"/>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.4">
-      <c r="D83" s="10"/>
-    </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.4">
-      <c r="D84" s="10"/>
-    </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.4">
-      <c r="D85" s="10"/>
-    </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.4">
-      <c r="D86" s="10"/>
-    </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.4">
-      <c r="D87" s="10"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="C85" s="9"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="C86" s="9"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+      <c r="C87" s="9"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="10"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="10"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="10"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="10"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="10"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="10"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:Q17" xr:uid="{F2FF41A7-1AA5-4667-B7A2-8D546222A2A4}"/>
+  <autoFilter ref="A4:R17" xr:uid="{F2FF41A7-1AA5-4667-B7A2-8D546222A2A4}"/>
   <mergeCells count="3">
     <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A19:J19"/>
-    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A49:J49"/>
   </mergeCells>
+  <conditionalFormatting sqref="P14:R21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2652,59 +3085,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481F2746-BDEC-4CBA-8D6B-10059F2652D1}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
+        <f>+'Data for Diji'!O5</f>
         <v>0.54172938773883617</v>
       </c>
       <c r="B2">
+        <f>+'Data for Diji'!O6</f>
         <v>0</v>
       </c>
       <c r="C2">
+        <f>+'Data for Diji'!O7</f>
         <v>2.5318034648191934E-2</v>
       </c>
       <c r="D2">
+        <f>+'Data for Diji'!O8</f>
         <v>0.11376517377271864</v>
       </c>
       <c r="E2">
+        <f>+'Data for Diji'!O9</f>
         <v>0.26657822761190836</v>
       </c>
       <c r="F2">
+        <f>+'Data for Diji'!O10</f>
         <v>5.4755282077962469E-4</v>
       </c>
       <c r="G2">
+        <f>+'Data for Diji'!O11</f>
         <v>9.0432763784842746E-3</v>
       </c>
       <c r="H2">
+        <f>+'Data for Diji'!O12</f>
         <v>4.3018347029080979E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed shared aras, added adjusted transition matrices, and added a nb that can be called to perform the adjustments
</commit_message>
<xml_diff>
--- a/ssp_modeling/scenario_mapping/Final scenario LULC areas_shared with SISEPUEDE.xlsx
+++ b/ssp_modeling/scenario_mapping/Final scenario LULC areas_shared with SISEPUEDE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fabian_fuentes\repos\ssp_uganda\ssp_modeling\scenario_mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/ssp_uganda/ssp_modeling/scenario_mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D2E687-2CE5-4D90-A6DB-D3AD954F606A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79C6B1D-00B1-C64E-B035-AB45581A3F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{2AEF5E3E-0A21-4B2E-B725-9AA9DDC8DE6E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="32260" windowHeight="18080" xr2:uid="{2AEF5E3E-0A21-4B2E-B725-9AA9DDC8DE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data for Diji" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="58">
   <si>
     <t>Seanrio LULC areas</t>
   </si>
@@ -203,12 +203,6 @@
     <t>SISEPUEDE</t>
   </si>
   <si>
-    <t>Primary forests</t>
-  </si>
-  <si>
-    <t>Secondary forests</t>
-  </si>
-  <si>
     <t>Name: 0, dtype: float64</t>
   </si>
   <si>
@@ -231,6 +225,9 @@
   </si>
   <si>
     <t>pij_lndu_grasslands_to_forests_primary</t>
+  </si>
+  <si>
+    <t>field_sisepuede</t>
   </si>
 </sst>
 </file>
@@ -242,8 +239,8 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
-    <numFmt numFmtId="172" formatCode="0.000000"/>
-    <numFmt numFmtId="173" formatCode="0.0000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -382,7 +379,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -431,16 +428,19 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -907,51 +907,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FF41A7-1AA5-4667-B7A2-8D546222A2A4}">
   <dimension ref="A1:V101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="32.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.375" customWidth="1"/>
-    <col min="4" max="4" width="18.375" customWidth="1"/>
-    <col min="5" max="5" width="18.625" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
-    <col min="7" max="10" width="16.75" customWidth="1"/>
-    <col min="12" max="12" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.375" customWidth="1"/>
-    <col min="14" max="14" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.625" customWidth="1"/>
-    <col min="16" max="16" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="10" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+    <row r="3" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-    </row>
-    <row r="4" spans="1:19" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+    </row>
+    <row r="4" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
@@ -981,6 +981,9 @@
       </c>
       <c r="J4" s="11" t="s">
         <v>11</v>
+      </c>
+      <c r="L4" s="47" t="s">
+        <v>57</v>
       </c>
       <c r="M4" s="36" t="s">
         <v>48</v>
@@ -999,7 +1002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1041,27 +1044,27 @@
         <v>0.167434</v>
       </c>
       <c r="N5" s="34">
-        <f>+G5+G12+G13</f>
-        <v>0.54172938773883617</v>
+        <f>+G12+G13</f>
+        <v>0.52563877698860129</v>
       </c>
       <c r="O5" s="34">
         <f>+N5</f>
-        <v>0.54172938773883617</v>
+        <v>0.52563877698860129</v>
       </c>
       <c r="P5" s="34">
-        <f>+H5+H12+H13</f>
-        <v>0.59798792185905869</v>
+        <f>+H12+H13</f>
+        <v>0.56797725489639994</v>
       </c>
       <c r="Q5" s="34">
-        <f>+I5+I12+I13</f>
-        <v>0.67211360620840199</v>
+        <f>+I12+I13</f>
+        <v>0.61922439470548984</v>
       </c>
       <c r="R5" s="34">
-        <f>+J5+J12+J13</f>
-        <v>0.78792287693961527</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <f>+J12+J13</f>
+        <v>0.69473286266790579</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1155,7 +1158,7 @@
         <v>3.9823217161954255E-3</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="M7" s="19">
         <v>0.49474299999999999</v>
@@ -1181,7 +1184,7 @@
         <v>2.2302888665755763E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1217,33 +1220,33 @@
         <v>4.9032094748936855E-2</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M8" s="26">
         <v>2.0045E-2</v>
       </c>
       <c r="N8" s="34">
-        <f>+G7+G8+G9</f>
-        <v>0.11376517377271864</v>
+        <f>+G5+G7+G8+G9</f>
+        <v>0.12985578452295354</v>
       </c>
       <c r="O8" s="34">
         <f t="shared" si="4"/>
-        <v>0.11376517377271864</v>
+        <v>0.12985578452295354</v>
       </c>
       <c r="P8" s="34">
-        <f>+H7+H8+H9</f>
-        <v>0.10131238113353408</v>
+        <f>+H5+H7+H8+H9</f>
+        <v>0.13132304809619286</v>
       </c>
       <c r="Q8" s="34">
-        <f>+I7+I8+I9</f>
-        <v>8.6864184358756133E-2</v>
+        <f>+I5+I7+I8+I9</f>
+        <v>0.13975339586166835</v>
       </c>
       <c r="R8" s="34">
-        <f>+J7+J8+J9</f>
-        <v>6.3665571213278135E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <f>+J5+J7+J8+J9</f>
+        <v>0.15685558548498754</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>9.5977820356562479E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1367,7 +1370,7 @@
         <v>5.4744151754816987E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>1.4775641130623662E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1492,7 +1495,7 @@
       </c>
       <c r="S12" s="41"/>
     </row>
-    <row r="13" spans="1:19" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1545,14 +1548,14 @@
       </c>
       <c r="Q13" s="35">
         <f t="shared" si="5"/>
-        <v>0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="R13" s="35">
         <f t="shared" si="5"/>
         <v>0.99979672603768843</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1595,18 +1598,18 @@
       <c r="O14" s="16"/>
       <c r="P14" s="34">
         <f t="shared" ref="P14:P21" si="6">+P5-N5</f>
-        <v>5.6258534120222525E-2</v>
+        <v>4.2338477907798655E-2</v>
       </c>
       <c r="Q14" s="34">
         <f>+Q5-P5</f>
-        <v>7.4125684349343302E-2</v>
+        <v>5.1247139809089903E-2</v>
       </c>
       <c r="R14" s="34">
         <f>+R5-Q5</f>
-        <v>0.11580927073121328</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+        <v>7.5508467962415948E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -1707,7 +1710,7 @@
         <v>-1.8820959768007482E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>25</v>
@@ -1736,18 +1739,18 @@
       <c r="O17" s="25"/>
       <c r="P17" s="34">
         <f t="shared" si="6"/>
-        <v>-1.2452792639184557E-2</v>
+        <v>1.4672635732393136E-3</v>
       </c>
       <c r="Q17" s="34">
         <f t="shared" si="7"/>
-        <v>-1.4448196774777947E-2</v>
+        <v>8.4303477654754932E-3</v>
       </c>
       <c r="R17" s="34">
         <f t="shared" ref="R17" si="10">+R8-Q8</f>
-        <v>-2.3198613145477998E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+        <v>1.7102189623319192E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1778,7 +1781,7 @@
         <v>2.24E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1802,13 +1805,13 @@
         <v>-1.1130323145482415E-7</v>
       </c>
       <c r="T19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="U19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1832,13 +1835,13 @@
         <v>1.8471259165717298E-3</v>
       </c>
       <c r="T20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="U20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1862,7 +1865,7 @@
         <v>-1.6060672131291365E-2</v>
       </c>
       <c r="T21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U21">
         <v>2.1220000000000002E-3</v>
@@ -1872,14 +1875,14 @@
         <v>2.1220000000000002E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="P22" s="34"/>
       <c r="T22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U22">
         <v>0</v>
@@ -1888,7 +1891,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1897,26 +1900,26 @@
         <v>47</v>
       </c>
       <c r="N23" s="35"/>
-      <c r="P23" s="45">
+      <c r="P23" s="43">
         <f>100%+P18</f>
         <v>0.95605348297234438</v>
       </c>
-      <c r="Q23" s="45">
+      <c r="Q23" s="43">
         <f>100%+Q18</f>
         <v>0.95006428782560459</v>
       </c>
-      <c r="R23" s="45">
+      <c r="R23" s="43">
         <f>100%+R18</f>
         <v>0.92328182194670516</v>
       </c>
       <c r="T23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1925,7 +1928,7 @@
         <v>40</v>
       </c>
       <c r="T24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="U24">
         <v>0.99765400000000004</v>
@@ -1935,7 +1938,7 @@
         <v>0.49765400000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1943,15 +1946,15 @@
       <c r="L25" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="S25" s="46"/>
+      <c r="S25" s="44"/>
       <c r="T25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="U25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1959,12 +1962,12 @@
       <c r="L26" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="P26" s="44"/>
+      <c r="P26" s="42"/>
       <c r="T26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1973,7 +1976,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1982,7 +1985,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1991,7 +1994,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -2000,33 +2003,33 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
+    <row r="33" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-    </row>
-    <row r="34" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+    </row>
+    <row r="34" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>2</v>
       </c>
@@ -2058,7 +2061,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>3.2684086987762935E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>3</v>
       </c>
@@ -2130,7 +2133,7 @@
         <v>0.11819901811538638</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>4</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>7.495079601702319E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>5</v>
       </c>
@@ -2202,7 +2205,7 @@
         <v>8.3632715922486625E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>6</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>1.8651779334038714E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>7</v>
       </c>
@@ -2274,7 +2277,7 @@
         <v>0.17682287685650652</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>8</v>
       </c>
@@ -2310,7 +2313,7 @@
         <v>5.7981380046387331E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>9</v>
       </c>
@@ -2346,7 +2349,7 @@
         <v>0.41071181427975628</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>10</v>
       </c>
@@ -2382,7 +2385,7 @@
         <v>7.8290932363106747E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>11</v>
       </c>
@@ -2418,7 +2421,7 @@
         <v>1.4779601013006356E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>12</v>
       </c>
@@ -2450,7 +2453,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>13</v>
       </c>
@@ -2486,7 +2489,7 @@
         <v>5.4744151754816987E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
       <c r="B47" s="5" t="s">
         <v>25</v>
@@ -2508,27 +2511,27 @@
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="42" t="s">
+    <row r="49" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A49" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
-      <c r="J49" s="42"/>
-    </row>
-    <row r="50" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+    </row>
+    <row r="50" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>2</v>
       </c>
@@ -2560,7 +2563,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>1</v>
       </c>
@@ -2596,7 +2599,7 @@
         <v>2.9726201510201365E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>3</v>
       </c>
@@ -2632,7 +2635,7 @@
         <v>0.12298891140046715</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>4</v>
       </c>
@@ -2668,7 +2671,7 @@
         <v>7.5129235161428519E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>5</v>
       </c>
@@ -2704,7 +2707,7 @@
         <v>8.3639609051078714E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>6</v>
       </c>
@@ -2740,7 +2743,7 @@
         <v>2.1774562136005534E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>7</v>
       </c>
@@ -2776,7 +2779,7 @@
         <v>0.23723318031402649</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>8</v>
       </c>
@@ -2812,7 +2815,7 @@
         <v>6.2827640546125468E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>9</v>
       </c>
@@ -2848,7 +2851,7 @@
         <v>0.33234158649412204</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>10</v>
       </c>
@@ -2884,7 +2887,7 @@
         <v>7.9378335620369112E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>11</v>
       </c>
@@ -2920,7 +2923,7 @@
         <v>2.2029559006476265E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>12</v>
       </c>
@@ -2952,7 +2955,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>13</v>
       </c>
@@ -2988,7 +2991,7 @@
         <v>5.4749040498499322E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
         <v>25</v>
@@ -3010,51 +3013,51 @@
       <c r="I63" s="8"/>
       <c r="J63" s="8"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="C85" s="9"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="C86" s="9"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="C87" s="9"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D101" s="10"/>
     </row>
   </sheetData>
@@ -3089,19 +3092,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>47</v>
       </c>
@@ -3127,10 +3130,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>+'Data for Diji'!O5</f>
-        <v>0.54172938773883617</v>
+        <v>0.52563877698860129</v>
       </c>
       <c r="B2">
         <f>+'Data for Diji'!O6</f>
@@ -3142,7 +3145,7 @@
       </c>
       <c r="D2">
         <f>+'Data for Diji'!O8</f>
-        <v>0.11376517377271864</v>
+        <v>0.12985578452295354</v>
       </c>
       <c r="E2">
         <f>+'Data for Diji'!O9</f>

</xml_diff>